<commit_message>
Credit Crad updated journey
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/CreditRegistration.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/CreditRegistration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-6220\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-8262020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,149 +24,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Case</t>
   </si>
   <si>
-    <t>CNIC_C</t>
-  </si>
-  <si>
-    <t>credit_card_no</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>Login_id</t>
   </si>
   <si>
     <t>scroll_text</t>
   </si>
   <si>
-    <t>When I am verifying Credit Sign up process 4220106968337</t>
-  </si>
-  <si>
-    <t>4220106968337</t>
-  </si>
-  <si>
-    <t>4902870003792964</t>
-  </si>
-  <si>
     <t>usman.safder@hbl.com</t>
   </si>
   <si>
-    <t>abbyabby124</t>
-  </si>
-  <si>
     <t>pakistan1</t>
   </si>
   <si>
-    <t>password_query</t>
-  </si>
-  <si>
     <t xml:space="preserve">13.6 </t>
   </si>
   <si>
     <t>customer_type_query</t>
   </si>
   <si>
-    <t>select P.CUSTOMER_TYPE from dc_customer_info P where P.CNIC ='4220106968337'</t>
-  </si>
-  <si>
-    <t>new_password</t>
-  </si>
-  <si>
     <t>success_message</t>
   </si>
   <si>
-    <t>account_query</t>
-  </si>
-  <si>
     <t>feedback_option</t>
   </si>
   <si>
-    <t>password_change_req_query</t>
-  </si>
-  <si>
     <t>transaction_password_query</t>
   </si>
   <si>
-    <t>Your Login password and Transaction password have been changed.Please login with new password</t>
-  </si>
-  <si>
-    <t>select ACCOUNT_NO  from dc_customer_account k where K.CUSTOMER_INFO_ID= ( Select customer_info_id from dc_customer_info i where I.CNIC='{customer_cnic}') AND K.IS_ACCOUNT_LINK='1'</t>
-  </si>
-  <si>
-    <t>select IS_PASSWORD_CHANGED_REQUIRED from dc_customer_info P where P.CNIC ='{customer_cnic}'</t>
-  </si>
-  <si>
     <t>select TRANSACTION_PASSWORD from dc_customer_info P where P.CNIC ='{customer_cnic}'</t>
   </si>
   <si>
     <t>pakistan2</t>
   </si>
   <si>
-    <t>activation_password</t>
-  </si>
-  <si>
-    <t>success_message1</t>
-  </si>
-  <si>
-    <t>success_message2</t>
-  </si>
-  <si>
-    <t>success_message3</t>
-  </si>
-  <si>
-    <t>You have registered successfully!</t>
-  </si>
-  <si>
-    <t>Your transaction has been processed successfully</t>
-  </si>
-  <si>
-    <t>Please note that you can use the same credentials to login on HBL Mobile.</t>
-  </si>
-  <si>
-    <t>Begin update dc_customer_info p set P.LOGIN_PASSWORD='$2a$10$fZ3EqVq2W9QWb2silU6sVuDUr.2XrXNSHjU98hOuQsCE/Dr1oN6cy' where P.CNIC='{customer_cnic}';COMMIT;END;</t>
-  </si>
-  <si>
     <t>select CUSTOMER_NAME from dc_customer_info P where P.CNIC ='{customer_cnic}'</t>
   </si>
   <si>
     <t>feedback_type</t>
   </si>
   <si>
-    <t>Facebook</t>
-  </si>
-  <si>
     <t>login_id_query</t>
   </si>
   <si>
-    <t>CNIC</t>
-  </si>
-  <si>
-    <t>Credit Card Number</t>
-  </si>
-  <si>
-    <t>Email Address Registered with HBL</t>
-  </si>
-  <si>
-    <t>credit_req_text1</t>
-  </si>
-  <si>
-    <t>credit_req_text3</t>
-  </si>
-  <si>
-    <t>credit_req_text2</t>
-  </si>
-  <si>
-    <t>dvl_query</t>
-  </si>
-  <si>
-    <t>Select PARAMTER_VALUE from DC_APPLICATION_PARAM_DETAIL C where C.PARAMETER_NAME='GET_DATA_FROM_DVL'</t>
-  </si>
-  <si>
     <t>IVR_require_query</t>
   </si>
   <si>
@@ -218,16 +122,64 @@
     <t>Select Z.ENABLE_PSD from dc_customer_info Z where Z.CNIC ='{customer_cnic}'</t>
   </si>
   <si>
-    <t>dob</t>
-  </si>
-  <si>
     <t>password_policy_query</t>
   </si>
   <si>
-    <t>Select PARAMTER_VALUE from DC_APPLICATION_PARAM_DETAIL P where P.PARAMETER_NAME ='LOGIN_PSWD_POLICY_DESC'</t>
-  </si>
-  <si>
     <t>Last_login_query</t>
+  </si>
+  <si>
+    <t>CNIC_D</t>
+  </si>
+  <si>
+    <t>Credit_card_no</t>
+  </si>
+  <si>
+    <t>Customer_Email</t>
+  </si>
+  <si>
+    <t>OTP_Value</t>
+  </si>
+  <si>
+    <t>login_pass</t>
+  </si>
+  <si>
+    <t>tran_pass</t>
+  </si>
+  <si>
+    <t>tran_pass_encrypted_value</t>
+  </si>
+  <si>
+    <t>3520229025957</t>
+  </si>
+  <si>
+    <t>4902870005771602</t>
+  </si>
+  <si>
+    <t>MOJIZABIDI99</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Select PARAMTER_VALUE from DC_APPLICATION_PARAM_DETAIL P where P.PARAMETER_NAME ='LOGIN_AND_T_PWRD_DESC_BEFORE_LOGIN'</t>
+  </si>
+  <si>
+    <t>You have successfully set-up your Login and Transaction Passwords. Kindly use your new password to login.</t>
+  </si>
+  <si>
+    <t>$2a$31$33GicMJLAlIuV0UQKrwtNu/SYwpsYsVkGR4DDNJEN9iSUwWoZtETu</t>
+  </si>
+  <si>
+    <t>select P.CUSTOMER_TYPE from dc_customer_info P where P.CNIC ='{customer_cnic}'</t>
+  </si>
+  <si>
+    <t>HBL Staff</t>
+  </si>
+  <si>
+    <t>681168</t>
+  </si>
+  <si>
+    <t>When I am verifying Credit Sign up process mojizabidi99</t>
   </si>
 </sst>
 </file>
@@ -243,12 +195,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -268,20 +218,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -557,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,251 +527,194 @@
     <col min="1" max="1" width="53.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="164.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="91.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="177.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="93.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="84.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="75.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="115.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="103.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="84.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="75.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="75.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="76" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="45.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="67.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="76.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="110.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="103.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="76.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="70.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="72.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="72.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="81.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="113" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="73" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="115.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="1"/>
+    <col min="19" max="19" width="72.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="72.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="70.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="81.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="113" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="73" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
+      <c r="K2" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="Y2" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB2" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J8:J12">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Excel Files Updated for Send Money (For Naeem)
</commit_message>
<xml_diff>
--- a/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/CreditRegistration.xlsx
+++ b/HBLAutomationWeb/Resources/Feature/InternetBanking/Data/CreditRegistration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-8262020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBL-Automation-9242020\HBLAutomationWeb\Resources\Feature\InternetBanking\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>